<commit_message>
update the log write mode
</commit_message>
<xml_diff>
--- a/result/gr100_010_simulated/details.xlsx
+++ b/result/gr100_010_simulated/details.xlsx
@@ -570,73 +570,73 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>0.8899774551391602</v>
+        <v>0.8136575222015381</v>
       </c>
       <c r="D2" t="n">
         <v>1</v>
       </c>
       <c r="E2" t="n">
-        <v>5306.59502012749</v>
+        <v>5251.587009206085</v>
       </c>
       <c r="F2" t="n">
         <v>0.1891980473820531</v>
       </c>
       <c r="G2" t="n">
-        <v>0.1761133153176759</v>
+        <v>0.1768077525252375</v>
       </c>
       <c r="H2" t="n">
-        <v>0.1743703669961806</v>
+        <v>0.1562931651970017</v>
       </c>
       <c r="I2" t="n">
-        <v>0.1738301466710666</v>
+        <v>0.1290241462329322</v>
       </c>
       <c r="J2" t="n">
-        <v>0.1631158790673703</v>
+        <v>0.1222519465937708</v>
       </c>
       <c r="K2" t="n">
-        <v>0.1458300740465699</v>
+        <v>0.1123494783187909</v>
       </c>
       <c r="L2" t="n">
-        <v>0.1383119220991934</v>
+        <v>0.110599287216326</v>
       </c>
       <c r="M2" t="n">
-        <v>0.1256346983275014</v>
+        <v>0.110599287216326</v>
       </c>
       <c r="N2" t="n">
-        <v>0.1179255815409161</v>
+        <v>0.110599287216326</v>
       </c>
       <c r="O2" t="n">
-        <v>0.1149737768068756</v>
+        <v>0.110599287216326</v>
       </c>
       <c r="P2" t="n">
-        <v>0.1123899317772846</v>
+        <v>0.110599287216326</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.1123899317772846</v>
+        <v>0.110599287216326</v>
       </c>
       <c r="R2" t="n">
-        <v>0.1118019996729461</v>
+        <v>0.110599287216326</v>
       </c>
       <c r="S2" t="n">
-        <v>0.1118019996729461</v>
+        <v>0.110599287216326</v>
       </c>
       <c r="T2" t="n">
-        <v>0.1116610461649002</v>
+        <v>0.110599287216326</v>
       </c>
       <c r="U2" t="n">
-        <v>0.1114423980531674</v>
+        <v>0.110599287216326</v>
       </c>
       <c r="V2" t="n">
-        <v>0.1114423980531674</v>
+        <v>0.1104908180339059</v>
       </c>
       <c r="W2" t="n">
-        <v>0.1114423980531674</v>
+        <v>0.1103991267324654</v>
       </c>
       <c r="X2" t="n">
-        <v>0.1114423980531674</v>
+        <v>0.1103990078872424</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.1114423980531674</v>
+        <v>0.1103701171385202</v>
       </c>
     </row>
     <row r="3">
@@ -649,13 +649,13 @@
         <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>0.8340005874633789</v>
+        <v>0.9103384017944336</v>
       </c>
       <c r="D3" t="n">
         <v>1</v>
       </c>
       <c r="E3" t="n">
-        <v>5247.549041465985</v>
+        <v>5239.93958471834</v>
       </c>
       <c r="F3" t="n">
         <v>0.1891980473820531</v>
@@ -664,58 +664,58 @@
         <v>0.1768077525252375</v>
       </c>
       <c r="H3" t="n">
-        <v>0.1704768560393269</v>
+        <v>0.161455175852402</v>
       </c>
       <c r="I3" t="n">
-        <v>0.1579184372511001</v>
+        <v>0.1486736310454331</v>
       </c>
       <c r="J3" t="n">
-        <v>0.1352773285118431</v>
+        <v>0.1348145567558006</v>
       </c>
       <c r="K3" t="n">
-        <v>0.128585687214688</v>
+        <v>0.1226590852641088</v>
       </c>
       <c r="L3" t="n">
-        <v>0.1172426569192755</v>
+        <v>0.1113589360804189</v>
       </c>
       <c r="M3" t="n">
-        <v>0.1122276633045169</v>
+        <v>0.1113589360804189</v>
       </c>
       <c r="N3" t="n">
-        <v>0.1114364253754302</v>
+        <v>0.1113589360804189</v>
       </c>
       <c r="O3" t="n">
-        <v>0.1112481185018588</v>
+        <v>0.1103713752629462</v>
       </c>
       <c r="P3" t="n">
-        <v>0.1112481185018588</v>
+        <v>0.1103713752629462</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.1110040714986633</v>
+        <v>0.1103423393696575</v>
       </c>
       <c r="R3" t="n">
-        <v>0.1102914043170757</v>
+        <v>0.1103423393696575</v>
       </c>
       <c r="S3" t="n">
-        <v>0.1102914043170757</v>
+        <v>0.1103423393696575</v>
       </c>
       <c r="T3" t="n">
-        <v>0.1102914043170757</v>
+        <v>0.1103423393696575</v>
       </c>
       <c r="U3" t="n">
-        <v>0.1102914043170757</v>
+        <v>0.1102899996290927</v>
       </c>
       <c r="V3" t="n">
-        <v>0.1102914043170757</v>
+        <v>0.1101836109344095</v>
       </c>
       <c r="W3" t="n">
-        <v>0.1102914043170757</v>
+        <v>0.1101430718268682</v>
       </c>
       <c r="X3" t="n">
-        <v>0.1102914043170757</v>
+        <v>0.1101430718268682</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.1102914043170757</v>
+        <v>0.1101430718268682</v>
       </c>
     </row>
     <row r="4">
@@ -728,73 +728,73 @@
         <v>2</v>
       </c>
       <c r="C4" t="n">
-        <v>0.8000154495239258</v>
+        <v>0.7541248798370361</v>
       </c>
       <c r="D4" t="n">
         <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>5271.960079096023</v>
+        <v>5304.026819530659</v>
       </c>
       <c r="F4" t="n">
         <v>0.1891980473820531</v>
       </c>
       <c r="G4" t="n">
-        <v>0.1768077525252375</v>
+        <v>0.1759815178231892</v>
       </c>
       <c r="H4" t="n">
-        <v>0.1639778095945271</v>
+        <v>0.1704439649691365</v>
       </c>
       <c r="I4" t="n">
-        <v>0.1556951294510229</v>
+        <v>0.1544716043545507</v>
       </c>
       <c r="J4" t="n">
-        <v>0.152001546185512</v>
+        <v>0.1390253213103271</v>
       </c>
       <c r="K4" t="n">
-        <v>0.1341887123125861</v>
+        <v>0.1257649309364189</v>
       </c>
       <c r="L4" t="n">
-        <v>0.1293309166155033</v>
+        <v>0.1163983791333658</v>
       </c>
       <c r="M4" t="n">
-        <v>0.1194490201005406</v>
+        <v>0.1145779466688847</v>
       </c>
       <c r="N4" t="n">
-        <v>0.1155511573708553</v>
+        <v>0.1132396693616662</v>
       </c>
       <c r="O4" t="n">
-        <v>0.1123801126085999</v>
+        <v>0.1119939767195134</v>
       </c>
       <c r="P4" t="n">
-        <v>0.1111817253358542</v>
+        <v>0.1119939767195134</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.1111817253358542</v>
+        <v>0.1114476863465585</v>
       </c>
       <c r="R4" t="n">
-        <v>0.1111817253358542</v>
+        <v>0.1114476863465585</v>
       </c>
       <c r="S4" t="n">
-        <v>0.1111740580115059</v>
+        <v>0.1114476863465585</v>
       </c>
       <c r="T4" t="n">
-        <v>0.1110030300628368</v>
+        <v>0.1114476863465585</v>
       </c>
       <c r="U4" t="n">
-        <v>0.1110030300628368</v>
+        <v>0.1114476863465585</v>
       </c>
       <c r="V4" t="n">
-        <v>0.1109118645015973</v>
+        <v>0.1114476863465585</v>
       </c>
       <c r="W4" t="n">
-        <v>0.1108691168322149</v>
+        <v>0.1114476863465585</v>
       </c>
       <c r="X4" t="n">
-        <v>0.1108691168322149</v>
+        <v>0.1114476863465585</v>
       </c>
       <c r="Y4" t="n">
-        <v>0.1107672530038211</v>
+        <v>0.1113923356633656</v>
       </c>
     </row>
     <row r="5">
@@ -807,13 +807,13 @@
         <v>3</v>
       </c>
       <c r="C5" t="n">
-        <v>0.7689990997314453</v>
+        <v>0.7812647819519043</v>
       </c>
       <c r="D5" t="n">
         <v>1</v>
       </c>
       <c r="E5" t="n">
-        <v>5230.510656730942</v>
+        <v>5293.157002932115</v>
       </c>
       <c r="F5" t="n">
         <v>0.1891980473820531</v>
@@ -822,58 +822,58 @@
         <v>0.1768077525252375</v>
       </c>
       <c r="H5" t="n">
-        <v>0.161550863640209</v>
+        <v>0.1738735936497511</v>
       </c>
       <c r="I5" t="n">
-        <v>0.1370623616671985</v>
+        <v>0.1640136354308318</v>
       </c>
       <c r="J5" t="n">
-        <v>0.1289248931765642</v>
+        <v>0.1557803293636605</v>
       </c>
       <c r="K5" t="n">
-        <v>0.1216496121012237</v>
+        <v>0.1557803293636605</v>
       </c>
       <c r="L5" t="n">
-        <v>0.1128396037707084</v>
+        <v>0.1421768380445265</v>
       </c>
       <c r="M5" t="n">
-        <v>0.1128396037707084</v>
+        <v>0.1306525455061247</v>
       </c>
       <c r="N5" t="n">
-        <v>0.1100590823768038</v>
+        <v>0.1200884781812499</v>
       </c>
       <c r="O5" t="n">
-        <v>0.110055356544349</v>
+        <v>0.1142164567146343</v>
       </c>
       <c r="P5" t="n">
-        <v>0.110055356544349</v>
+        <v>0.1128810015160823</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.110055356544349</v>
+        <v>0.1128810015160823</v>
       </c>
       <c r="R5" t="n">
-        <v>0.110055356544349</v>
+        <v>0.1128810015160823</v>
       </c>
       <c r="S5" t="n">
-        <v>0.110055356544349</v>
+        <v>0.1124969977363263</v>
       </c>
       <c r="T5" t="n">
-        <v>0.110055356544349</v>
+        <v>0.1120218462609039</v>
       </c>
       <c r="U5" t="n">
-        <v>0.110055356544349</v>
+        <v>0.112006882364714</v>
       </c>
       <c r="V5" t="n">
-        <v>0.109959272061032</v>
+        <v>0.1113745270724463</v>
       </c>
       <c r="W5" t="n">
-        <v>0.109959272061032</v>
+        <v>0.1113745270724463</v>
       </c>
       <c r="X5" t="n">
-        <v>0.109959272061032</v>
+        <v>0.1113199543587014</v>
       </c>
       <c r="Y5" t="n">
-        <v>0.109959272061032</v>
+        <v>0.1111804484002361</v>
       </c>
     </row>
     <row r="6">
@@ -886,73 +886,73 @@
         <v>4</v>
       </c>
       <c r="C6" t="n">
-        <v>0.7960271835327148</v>
+        <v>0.7500004768371582</v>
       </c>
       <c r="D6" t="n">
         <v>1</v>
       </c>
       <c r="E6" t="n">
-        <v>5299.445650310915</v>
+        <v>5303.964419364228</v>
       </c>
       <c r="F6" t="n">
         <v>0.1891980473820531</v>
       </c>
       <c r="G6" t="n">
-        <v>0.1768077525252375</v>
+        <v>0.1755357036184034</v>
       </c>
       <c r="H6" t="n">
-        <v>0.1589949275798517</v>
+        <v>0.1640697804787035</v>
       </c>
       <c r="I6" t="n">
-        <v>0.148149440990216</v>
+        <v>0.1589793087751172</v>
       </c>
       <c r="J6" t="n">
-        <v>0.1380740795215327</v>
+        <v>0.1345595289219969</v>
       </c>
       <c r="K6" t="n">
-        <v>0.117878843309816</v>
+        <v>0.1216186440732276</v>
       </c>
       <c r="L6" t="n">
-        <v>0.1139725624340961</v>
+        <v>0.120186986720946</v>
       </c>
       <c r="M6" t="n">
-        <v>0.1121747837437453</v>
+        <v>0.1136580202055247</v>
       </c>
       <c r="N6" t="n">
-        <v>0.1121747837437453</v>
+        <v>0.1132763573958065</v>
       </c>
       <c r="O6" t="n">
-        <v>0.1117625489145448</v>
+        <v>0.1129269425250347</v>
       </c>
       <c r="P6" t="n">
-        <v>0.1117276043420562</v>
+        <v>0.1122000285980301</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.1116387471216536</v>
+        <v>0.1116684679781859</v>
       </c>
       <c r="R6" t="n">
-        <v>0.1115965426870993</v>
+        <v>0.1116684679781859</v>
       </c>
       <c r="S6" t="n">
-        <v>0.1114404499217894</v>
+        <v>0.1116684679781859</v>
       </c>
       <c r="T6" t="n">
-        <v>0.1114404499217894</v>
+        <v>0.1115941094021108</v>
       </c>
       <c r="U6" t="n">
-        <v>0.1114404499217894</v>
+        <v>0.1115527727625577</v>
       </c>
       <c r="V6" t="n">
-        <v>0.1114404499217894</v>
+        <v>0.1115208954649315</v>
       </c>
       <c r="W6" t="n">
-        <v>0.1113030341191211</v>
+        <v>0.1114988199640495</v>
       </c>
       <c r="X6" t="n">
-        <v>0.1113030341191211</v>
+        <v>0.1113911192858524</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.1113030341191211</v>
+        <v>0.1113911192858524</v>
       </c>
     </row>
     <row r="7">
@@ -965,73 +965,73 @@
         <v>5</v>
       </c>
       <c r="C7" t="n">
-        <v>0.8029744625091553</v>
+        <v>0.7656099796295166</v>
       </c>
       <c r="D7" t="n">
         <v>1</v>
       </c>
       <c r="E7" t="n">
-        <v>5434.127413751195</v>
+        <v>5282.017459606802</v>
       </c>
       <c r="F7" t="n">
         <v>0.1891980473820531</v>
       </c>
       <c r="G7" t="n">
-        <v>0.1768077525252375</v>
+        <v>0.1766969141991905</v>
       </c>
       <c r="H7" t="n">
-        <v>0.167935995496463</v>
+        <v>0.164316411212265</v>
       </c>
       <c r="I7" t="n">
-        <v>0.1631528455778617</v>
+        <v>0.1598154972331221</v>
       </c>
       <c r="J7" t="n">
-        <v>0.1613030867172744</v>
+        <v>0.1406437875633592</v>
       </c>
       <c r="K7" t="n">
-        <v>0.1419089019283254</v>
+        <v>0.1247041553975499</v>
       </c>
       <c r="L7" t="n">
-        <v>0.1290056062631035</v>
+        <v>0.121775693362497</v>
       </c>
       <c r="M7" t="n">
-        <v>0.123250113214338</v>
+        <v>0.11621524269717</v>
       </c>
       <c r="N7" t="n">
-        <v>0.1178165077004984</v>
+        <v>0.1159997839105884</v>
       </c>
       <c r="O7" t="n">
-        <v>0.1155271789751819</v>
+        <v>0.1131130031751423</v>
       </c>
       <c r="P7" t="n">
-        <v>0.11399917999028</v>
+        <v>0.1119299582326765</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.11399917999028</v>
+        <v>0.111527804651788</v>
       </c>
       <c r="R7" t="n">
-        <v>0.11399917999028</v>
+        <v>0.1111136819958433</v>
       </c>
       <c r="S7" t="n">
-        <v>0.11399917999028</v>
+        <v>0.1111136819958433</v>
       </c>
       <c r="T7" t="n">
-        <v>0.11399917999028</v>
+        <v>0.1111136819958433</v>
       </c>
       <c r="U7" t="n">
-        <v>0.11399917999028</v>
+        <v>0.1111136819958433</v>
       </c>
       <c r="V7" t="n">
-        <v>0.11399917999028</v>
+        <v>0.1110170965579736</v>
       </c>
       <c r="W7" t="n">
-        <v>0.11399917999028</v>
+        <v>0.1110170965579736</v>
       </c>
       <c r="X7" t="n">
-        <v>0.1139806209278305</v>
+        <v>0.1109633033061755</v>
       </c>
       <c r="Y7" t="n">
-        <v>0.1139284096247796</v>
+        <v>0.1109633033061755</v>
       </c>
     </row>
     <row r="8">
@@ -1044,73 +1044,73 @@
         <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>0.780038595199585</v>
+        <v>0.7656407356262207</v>
       </c>
       <c r="D8" t="n">
         <v>1</v>
       </c>
       <c r="E8" t="n">
-        <v>5294.206649995872</v>
+        <v>5220.411555874026</v>
       </c>
       <c r="F8" t="n">
         <v>0.1891980473820531</v>
       </c>
       <c r="G8" t="n">
-        <v>0.1768077525252375</v>
+        <v>0.176567158427775</v>
       </c>
       <c r="H8" t="n">
-        <v>0.1743703669961806</v>
+        <v>0.1704988410581034</v>
       </c>
       <c r="I8" t="n">
-        <v>0.1428764251484767</v>
+        <v>0.1667848578834215</v>
       </c>
       <c r="J8" t="n">
-        <v>0.1276745995954535</v>
+        <v>0.1600783451254889</v>
       </c>
       <c r="K8" t="n">
-        <v>0.1214047005319449</v>
+        <v>0.1462654811072261</v>
       </c>
       <c r="L8" t="n">
-        <v>0.1148582617813248</v>
+        <v>0.1362902297613469</v>
       </c>
       <c r="M8" t="n">
-        <v>0.1125919045227397</v>
+        <v>0.1238884089341805</v>
       </c>
       <c r="N8" t="n">
-        <v>0.1123945255024498</v>
+        <v>0.1202695018986898</v>
       </c>
       <c r="O8" t="n">
-        <v>0.1123945255024498</v>
+        <v>0.1122873479151376</v>
       </c>
       <c r="P8" t="n">
-        <v>0.1120107030553845</v>
+        <v>0.1122873479151376</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.1120107030553845</v>
+        <v>0.1119152366555455</v>
       </c>
       <c r="R8" t="n">
-        <v>0.1114198609015387</v>
+        <v>0.1099923808320071</v>
       </c>
       <c r="S8" t="n">
-        <v>0.1114198609015387</v>
+        <v>0.1099923808320071</v>
       </c>
       <c r="T8" t="n">
-        <v>0.1114198609015387</v>
+        <v>0.1099923808320071</v>
       </c>
       <c r="U8" t="n">
-        <v>0.1113645008857076</v>
+        <v>0.1099923808320071</v>
       </c>
       <c r="V8" t="n">
-        <v>0.1113645008857076</v>
+        <v>0.1099749872789408</v>
       </c>
       <c r="W8" t="n">
-        <v>0.1113645008857076</v>
+        <v>0.1098886644941043</v>
       </c>
       <c r="X8" t="n">
-        <v>0.1112064409975845</v>
+        <v>0.109857368169683</v>
       </c>
       <c r="Y8" t="n">
-        <v>0.1112009093566446</v>
+        <v>0.1097624084965697</v>
       </c>
     </row>
     <row r="9">
@@ -1123,13 +1123,13 @@
         <v>7</v>
       </c>
       <c r="C9" t="n">
-        <v>0.8149607181549072</v>
+        <v>0.7656099796295166</v>
       </c>
       <c r="D9" t="n">
         <v>1</v>
       </c>
       <c r="E9" t="n">
-        <v>5234.376103185858</v>
+        <v>5346.633874085862</v>
       </c>
       <c r="F9" t="n">
         <v>0.1891980473820531</v>
@@ -1138,58 +1138,58 @@
         <v>0.1768077525252375</v>
       </c>
       <c r="H9" t="n">
-        <v>0.150053212271294</v>
+        <v>0.1681031536281684</v>
       </c>
       <c r="I9" t="n">
-        <v>0.1327873090411359</v>
+        <v>0.1635900573481348</v>
       </c>
       <c r="J9" t="n">
-        <v>0.1139519871458935</v>
+        <v>0.1630397854576907</v>
       </c>
       <c r="K9" t="n">
-        <v>0.1126153295587546</v>
+        <v>0.1628980015650583</v>
       </c>
       <c r="L9" t="n">
-        <v>0.1116344768146588</v>
+        <v>0.1495247239398385</v>
       </c>
       <c r="M9" t="n">
-        <v>0.1115582477783175</v>
+        <v>0.1366424751627321</v>
       </c>
       <c r="N9" t="n">
-        <v>0.110776739150528</v>
+        <v>0.131222699331177</v>
       </c>
       <c r="O9" t="n">
-        <v>0.1105795701762201</v>
+        <v>0.1212398755191479</v>
       </c>
       <c r="P9" t="n">
-        <v>0.1105795701762201</v>
+        <v>0.1155117876191576</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.1104892356460894</v>
+        <v>0.1134719572696688</v>
       </c>
       <c r="R9" t="n">
-        <v>0.1104892356460894</v>
+        <v>0.1132678214429601</v>
       </c>
       <c r="S9" t="n">
-        <v>0.1100346218944611</v>
+        <v>0.1131124102144254</v>
       </c>
       <c r="T9" t="n">
-        <v>0.1100346218944611</v>
+        <v>0.112862561058884</v>
       </c>
       <c r="U9" t="n">
-        <v>0.1100346218944611</v>
+        <v>0.1125381242188264</v>
       </c>
       <c r="V9" t="n">
-        <v>0.1100346218944611</v>
+        <v>0.1123776489882607</v>
       </c>
       <c r="W9" t="n">
-        <v>0.1100346218944611</v>
+        <v>0.1123776489882607</v>
       </c>
       <c r="X9" t="n">
-        <v>0.1100346218944611</v>
+        <v>0.1123364319059773</v>
       </c>
       <c r="Y9" t="n">
-        <v>0.1100346218944611</v>
+        <v>0.1122228825357868</v>
       </c>
     </row>
     <row r="10">
@@ -1202,73 +1202,73 @@
         <v>8</v>
       </c>
       <c r="C10" t="n">
-        <v>0.8020098209381104</v>
+        <v>0.7499711513519287</v>
       </c>
       <c r="D10" t="n">
         <v>1</v>
       </c>
       <c r="E10" t="n">
-        <v>5259.140879587797</v>
+        <v>5248.172324976495</v>
       </c>
       <c r="F10" t="n">
         <v>0.1891980473820531</v>
       </c>
       <c r="G10" t="n">
-        <v>0.1768077525252375</v>
+        <v>0.1749353116568467</v>
       </c>
       <c r="H10" t="n">
-        <v>0.159731950409196</v>
+        <v>0.1743703669961806</v>
       </c>
       <c r="I10" t="n">
-        <v>0.1339082859019534</v>
+        <v>0.153332217040805</v>
       </c>
       <c r="J10" t="n">
-        <v>0.1248429563872574</v>
+        <v>0.1404291122959017</v>
       </c>
       <c r="K10" t="n">
-        <v>0.1153549575858369</v>
+        <v>0.1223118898907158</v>
       </c>
       <c r="L10" t="n">
-        <v>0.1129103132616688</v>
+        <v>0.1174028565222355</v>
       </c>
       <c r="M10" t="n">
-        <v>0.1115989651536394</v>
+        <v>0.1123521752028529</v>
       </c>
       <c r="N10" t="n">
-        <v>0.1115989651536394</v>
+        <v>0.1118817752150991</v>
       </c>
       <c r="O10" t="n">
-        <v>0.1113775687464815</v>
+        <v>0.1118253108225645</v>
       </c>
       <c r="P10" t="n">
-        <v>0.1112057519766065</v>
+        <v>0.1106301945897721</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.1107241028132843</v>
+        <v>0.1106301945897721</v>
       </c>
       <c r="R10" t="n">
-        <v>0.1107241028132843</v>
+        <v>0.1103840750571846</v>
       </c>
       <c r="S10" t="n">
-        <v>0.1105224068322483</v>
+        <v>0.1103840750571846</v>
       </c>
       <c r="T10" t="n">
-        <v>0.1105224068322483</v>
+        <v>0.1103840750571846</v>
       </c>
       <c r="U10" t="n">
-        <v>0.1105224068322483</v>
+        <v>0.1103840750571846</v>
       </c>
       <c r="V10" t="n">
-        <v>0.1105224068322483</v>
+        <v>0.1103840750571846</v>
       </c>
       <c r="W10" t="n">
-        <v>0.1105224068322483</v>
+        <v>0.1103371037618439</v>
       </c>
       <c r="X10" t="n">
-        <v>0.1105224068322483</v>
+        <v>0.1103371037618439</v>
       </c>
       <c r="Y10" t="n">
-        <v>0.1105173660738362</v>
+        <v>0.110303554093109</v>
       </c>
     </row>
     <row r="11">
@@ -1281,73 +1281,73 @@
         <v>9</v>
       </c>
       <c r="C11" t="n">
-        <v>0.7850301265716553</v>
+        <v>0.8281238079071045</v>
       </c>
       <c r="D11" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E11" t="n">
-        <v>5232.932343226397</v>
+        <v>6979.274756502823</v>
       </c>
       <c r="F11" t="n">
         <v>0.1891980473820531</v>
       </c>
       <c r="G11" t="n">
-        <v>0.1746381459540055</v>
+        <v>0.1755590590951902</v>
       </c>
       <c r="H11" t="n">
-        <v>0.159792127442851</v>
+        <v>0.1668607725105126</v>
       </c>
       <c r="I11" t="n">
-        <v>0.1460431572011607</v>
+        <v>0.1610084600525325</v>
       </c>
       <c r="J11" t="n">
-        <v>0.1267376735055271</v>
+        <v>0.1603497614514845</v>
       </c>
       <c r="K11" t="n">
-        <v>0.119284061282125</v>
+        <v>0.1603497614514845</v>
       </c>
       <c r="L11" t="n">
-        <v>0.1136106320782341</v>
+        <v>0.1603497614514845</v>
       </c>
       <c r="M11" t="n">
-        <v>0.1136106320782341</v>
+        <v>0.1601369356677987</v>
       </c>
       <c r="N11" t="n">
-        <v>0.1114562972684715</v>
+        <v>0.1601369356677987</v>
       </c>
       <c r="O11" t="n">
-        <v>0.1114562972684715</v>
+        <v>0.1601369356677987</v>
       </c>
       <c r="P11" t="n">
-        <v>0.1111370409131377</v>
+        <v>0.1601369356677987</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.1107199494325045</v>
+        <v>0.1601369356677987</v>
       </c>
       <c r="R11" t="n">
-        <v>0.110136272771401</v>
+        <v>0.1601369356677987</v>
       </c>
       <c r="S11" t="n">
-        <v>0.1100064784254658</v>
+        <v>0.1601369356677987</v>
       </c>
       <c r="T11" t="n">
-        <v>0.1100064784254658</v>
+        <v>0.1601369356677987</v>
       </c>
       <c r="U11" t="n">
-        <v>0.1100064784254658</v>
+        <v>0.1601369356677987</v>
       </c>
       <c r="V11" t="n">
-        <v>0.1100064784254658</v>
+        <v>0.1601369356677987</v>
       </c>
       <c r="W11" t="n">
-        <v>0.1100064784254658</v>
+        <v>0.1601369356677987</v>
       </c>
       <c r="X11" t="n">
-        <v>0.1100064784254658</v>
+        <v>0.1601081527615442</v>
       </c>
       <c r="Y11" t="n">
-        <v>0.1100064784254658</v>
+        <v>0.1600482408675014</v>
       </c>
     </row>
   </sheetData>

</xml_diff>